<commit_message>
Solicitud gráfica y manuscrito 02 décimo, actualizados
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado10/guion02/SolicitudGrafica_CS_10_02_CO.xlsx
+++ b/fuentes/contenidos/grado10/guion02/SolicitudGrafica_CS_10_02_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zambanitos\Documents\MABEL\TRABAJO\PLANETA\REINGENIERIA_AGOSTO\CUADERNOS DE ESTUDIO\guion02\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zambanitos\Documents\GitHub\CienciasSociales\fuentes\contenidos\grado10\guion02\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="hX79YNGfHMUCcosWMoH0GQuhNo2gkebFrfW3do2TOcvwqaujU9m0uwOL5UkRtWEspAy/ISD2JB8+jf057W9mVA==" workbookSaltValue="uRz/CDpmZ5ecKheoN1C0Jw==" workbookSpinCount="100000" lockStructure="1"/>
@@ -1810,6 +1810,18 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="51" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="51"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1908,18 +1920,6 @@
     <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="51" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="51"/>
   </cellXfs>
   <cellStyles count="52">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -2757,7 +2757,7 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="140" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="140" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E10" sqref="E10:E50"/>
     </sheetView>
@@ -2805,14 +2805,14 @@
       <c r="B2" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="83" t="s">
+      <c r="C2" s="88" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="84"/>
-      <c r="F2" s="76" t="s">
+      <c r="D2" s="89"/>
+      <c r="F2" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="77"/>
+      <c r="G2" s="82"/>
       <c r="H2" s="58"/>
       <c r="I2" s="58"/>
       <c r="J2" s="14"/>
@@ -2836,14 +2836,14 @@
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="85">
+      <c r="C3" s="90">
         <v>10</v>
       </c>
-      <c r="D3" s="86"/>
-      <c r="F3" s="78">
+      <c r="D3" s="91"/>
+      <c r="F3" s="83">
         <v>42245</v>
       </c>
-      <c r="G3" s="79"/>
+      <c r="G3" s="84"/>
       <c r="H3" s="58"/>
       <c r="I3" s="38"/>
       <c r="J3" s="14"/>
@@ -2867,10 +2867,10 @@
       <c r="B4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="85" t="s">
+      <c r="C4" s="90" t="s">
         <v>187</v>
       </c>
-      <c r="D4" s="86"/>
+      <c r="D4" s="91"/>
       <c r="E4" s="5"/>
       <c r="F4" s="37" t="s">
         <v>55</v>
@@ -2899,10 +2899,10 @@
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="87" t="s">
+      <c r="C5" s="92" t="s">
         <v>188</v>
       </c>
-      <c r="D5" s="88"/>
+      <c r="D5" s="93"/>
       <c r="E5" s="5"/>
       <c r="F5" s="37" t="str">
         <f>IF(G4="Recurso","Motor del recurso","")</f>
@@ -2984,12 +2984,12 @@
       <c r="C8" s="9"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="80" t="s">
+      <c r="F8" s="85" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="81"/>
-      <c r="H8" s="81"/>
-      <c r="I8" s="82"/>
+      <c r="G8" s="86"/>
+      <c r="H8" s="86"/>
+      <c r="I8" s="87"/>
       <c r="J8" s="16"/>
       <c r="K8" s="11"/>
       <c r="M8" s="2" t="str">
@@ -3050,7 +3050,7 @@
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),"IMG01","")</f>
         <v>IMG01</v>
       </c>
-      <c r="B10" s="107" t="s">
+      <c r="B10" s="76" t="s">
         <v>191</v>
       </c>
       <c r="C10" s="20" t="str">
@@ -3079,7 +3079,7 @@
         <f ca="1">IF(OR($B10&lt;&gt;"",$J10&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E10,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E10,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J10" s="107" t="s">
+      <c r="J10" s="76" t="s">
         <v>192</v>
       </c>
       <c r="K10" s="64"/>
@@ -3093,7 +3093,7 @@
         <f t="shared" ref="A11:A18" si="3">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE(LEFT(A10,3),IF(MID(A10,4,2)+1&lt;10,CONCATENATE("0",MID(A10,4,2)+1))),"")</f>
         <v>IMG02</v>
       </c>
-      <c r="B11" s="107" t="s">
+      <c r="B11" s="76" t="s">
         <v>193</v>
       </c>
       <c r="C11" s="20" t="str">
@@ -3122,7 +3122,7 @@
         <f ca="1">IF(OR($B11&lt;&gt;"",$J11&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E11,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E11,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J11" s="107" t="s">
+      <c r="J11" s="76" t="s">
         <v>194</v>
       </c>
       <c r="K11" s="65"/>
@@ -3136,7 +3136,7 @@
         <f t="shared" si="3"/>
         <v>IMG03</v>
       </c>
-      <c r="B12" s="107" t="s">
+      <c r="B12" s="76" t="s">
         <v>195</v>
       </c>
       <c r="C12" s="20" t="str">
@@ -3165,7 +3165,7 @@
         <f ca="1">IF(OR($B12&lt;&gt;"",$J12&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E12,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E12,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J12" s="107" t="s">
+      <c r="J12" s="76" t="s">
         <v>196</v>
       </c>
       <c r="K12" s="64"/>
@@ -3179,7 +3179,7 @@
         <f t="shared" si="3"/>
         <v>IMG04</v>
       </c>
-      <c r="B13" s="108" t="s">
+      <c r="B13" s="77" t="s">
         <v>197</v>
       </c>
       <c r="C13" s="20" t="str">
@@ -3224,7 +3224,7 @@
         <f t="shared" si="3"/>
         <v>IMG05</v>
       </c>
-      <c r="B14" s="107" t="s">
+      <c r="B14" s="76" t="s">
         <v>200</v>
       </c>
       <c r="C14" s="20" t="str">
@@ -3267,7 +3267,7 @@
         <f t="shared" si="3"/>
         <v>IMG06</v>
       </c>
-      <c r="B15" s="107" t="s">
+      <c r="B15" s="76" t="s">
         <v>202</v>
       </c>
       <c r="C15" s="20" t="str">
@@ -3296,7 +3296,7 @@
         <f ca="1">IF(OR($B15&lt;&gt;"",$J15&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E15,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E15,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J15" s="107" t="s">
+      <c r="J15" s="76" t="s">
         <v>203</v>
       </c>
       <c r="K15" s="66"/>
@@ -3310,7 +3310,7 @@
         <f t="shared" si="3"/>
         <v>IMG07</v>
       </c>
-      <c r="B16" s="107" t="s">
+      <c r="B16" s="76" t="s">
         <v>204</v>
       </c>
       <c r="C16" s="20" t="str">
@@ -3353,7 +3353,7 @@
         <f t="shared" si="3"/>
         <v>IMG08</v>
       </c>
-      <c r="B17" s="107" t="s">
+      <c r="B17" s="76" t="s">
         <v>206</v>
       </c>
       <c r="C17" s="20" t="str">
@@ -3382,7 +3382,7 @@
         <f ca="1">IF(OR($B17&lt;&gt;"",$J17&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E17,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E17,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J17" s="107" t="s">
+      <c r="J17" s="76" t="s">
         <v>207</v>
       </c>
       <c r="K17" s="66"/>
@@ -3396,7 +3396,7 @@
         <f t="shared" si="3"/>
         <v>IMG09</v>
       </c>
-      <c r="B18" s="107" t="s">
+      <c r="B18" s="76" t="s">
         <v>208</v>
       </c>
       <c r="C18" s="20" t="str">
@@ -3439,7 +3439,7 @@
         <f t="shared" ref="A19:A50" si="6">IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),CONCATENATE(LEFT(A18,3),IF(MID(A18,4,2)+1&lt;10,CONCATENATE("0",MID(A18,4,2)+1),MID(A18,4,2)+1)),"")</f>
         <v>IMG10</v>
       </c>
-      <c r="B19" s="107" t="s">
+      <c r="B19" s="76" t="s">
         <v>210</v>
       </c>
       <c r="C19" s="20" t="str">
@@ -3468,7 +3468,7 @@
         <f ca="1">IF(OR($B19&lt;&gt;"",$J19&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E19,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E19,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J19" s="107" t="s">
+      <c r="J19" s="76" t="s">
         <v>211</v>
       </c>
       <c r="K19" s="68"/>
@@ -3482,7 +3482,7 @@
         <f t="shared" si="6"/>
         <v>IMG11</v>
       </c>
-      <c r="B20" s="107" t="s">
+      <c r="B20" s="76" t="s">
         <v>212</v>
       </c>
       <c r="C20" s="20" t="str">
@@ -3511,7 +3511,7 @@
         <f ca="1">IF(OR($B20&lt;&gt;"",$J20&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E20,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E20,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J20" s="107" t="s">
+      <c r="J20" s="76" t="s">
         <v>213</v>
       </c>
       <c r="K20" s="66"/>
@@ -3525,7 +3525,7 @@
         <f>IF(OR(B21&lt;&gt;"",K21&lt;&gt;""),CONCATENATE(LEFT(A20,3),IF(MID(A20,4,2)+1&lt;10,CONCATENATE("0",MID(A20,4,2)+1),MID(A20,4,2)+1)),"")</f>
         <v>IMG12</v>
       </c>
-      <c r="B21" s="109" t="s">
+      <c r="B21" s="78" t="s">
         <v>214</v>
       </c>
       <c r="C21" s="20" t="str">
@@ -3554,7 +3554,7 @@
         <f ca="1">IF(OR($B21&lt;&gt;"",$K21&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E21,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E21,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J21" s="110" t="s">
+      <c r="J21" s="79" t="s">
         <v>216</v>
       </c>
       <c r="K21" s="66" t="s">
@@ -3570,7 +3570,7 @@
         <f t="shared" si="6"/>
         <v>IMG13</v>
       </c>
-      <c r="B22" s="107" t="s">
+      <c r="B22" s="76" t="s">
         <v>217</v>
       </c>
       <c r="C22" s="20" t="str">
@@ -3599,7 +3599,7 @@
         <f ca="1">IF(OR($B22&lt;&gt;"",$J22&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E22,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E22,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J22" s="107" t="s">
+      <c r="J22" s="76" t="s">
         <v>218</v>
       </c>
       <c r="K22" s="69"/>
@@ -3613,7 +3613,7 @@
         <f t="shared" si="6"/>
         <v>IMG14</v>
       </c>
-      <c r="B23" s="107" t="s">
+      <c r="B23" s="76" t="s">
         <v>219</v>
       </c>
       <c r="C23" s="20" t="str">
@@ -3642,7 +3642,7 @@
         <f ca="1">IF(OR($B23&lt;&gt;"",$J23&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E23,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E23,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J23" s="107" t="s">
+      <c r="J23" s="76" t="s">
         <v>220</v>
       </c>
       <c r="K23" s="64"/>
@@ -3656,7 +3656,7 @@
         <f t="shared" si="6"/>
         <v>IMG15</v>
       </c>
-      <c r="B24" s="107" t="s">
+      <c r="B24" s="76" t="s">
         <v>221</v>
       </c>
       <c r="C24" s="20" t="str">
@@ -3685,7 +3685,7 @@
         <f ca="1">IF(OR($B24&lt;&gt;"",$J24&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E24,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E24,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J24" s="107" t="s">
+      <c r="J24" s="76" t="s">
         <v>222</v>
       </c>
       <c r="K24" s="65"/>
@@ -3699,7 +3699,7 @@
         <f t="shared" si="6"/>
         <v>IMG16</v>
       </c>
-      <c r="B25" s="107" t="s">
+      <c r="B25" s="76" t="s">
         <v>219</v>
       </c>
       <c r="C25" s="20" t="str">
@@ -3738,7 +3738,7 @@
         <f t="shared" si="6"/>
         <v>IMG17</v>
       </c>
-      <c r="B26" s="107" t="s">
+      <c r="B26" s="76" t="s">
         <v>224</v>
       </c>
       <c r="C26" s="20" t="str">
@@ -3767,7 +3767,7 @@
         <f ca="1">IF(OR($B26&lt;&gt;"",$J26&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E26,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E26,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J26" s="107" t="s">
+      <c r="J26" s="76" t="s">
         <v>225</v>
       </c>
       <c r="K26" s="64"/>
@@ -3777,7 +3777,7 @@
         <f t="shared" si="6"/>
         <v>IMG18</v>
       </c>
-      <c r="B27" s="107" t="s">
+      <c r="B27" s="76" t="s">
         <v>226</v>
       </c>
       <c r="C27" s="20" t="str">
@@ -3806,7 +3806,7 @@
         <f ca="1">IF(OR($B27&lt;&gt;"",$J27&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E27,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E27,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J27" s="107" t="s">
+      <c r="J27" s="76" t="s">
         <v>227</v>
       </c>
       <c r="K27" s="64"/>
@@ -3817,7 +3817,7 @@
         <f t="shared" si="6"/>
         <v>IMG19</v>
       </c>
-      <c r="B28" s="108" t="s">
+      <c r="B28" s="77" t="s">
         <v>228</v>
       </c>
       <c r="C28" s="20" t="str">
@@ -3858,7 +3858,7 @@
         <f t="shared" si="6"/>
         <v>IMG20</v>
       </c>
-      <c r="B29" s="107" t="s">
+      <c r="B29" s="76" t="s">
         <v>231</v>
       </c>
       <c r="C29" s="20" t="str">
@@ -3887,7 +3887,7 @@
         <f ca="1">IF(OR($B29&lt;&gt;"",$J29&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E29,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E29,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J29" s="107" t="s">
+      <c r="J29" s="76" t="s">
         <v>232</v>
       </c>
       <c r="K29" s="64"/>
@@ -3897,7 +3897,7 @@
         <f t="shared" si="6"/>
         <v>IMG21</v>
       </c>
-      <c r="B30" s="107" t="s">
+      <c r="B30" s="76" t="s">
         <v>233</v>
       </c>
       <c r="C30" s="20" t="str">
@@ -3926,7 +3926,7 @@
         <f ca="1">IF(OR($B30&lt;&gt;"",$J30&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E30,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E30,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J30" s="107" t="s">
+      <c r="J30" s="76" t="s">
         <v>234</v>
       </c>
       <c r="K30" s="64"/>
@@ -3936,7 +3936,7 @@
         <f t="shared" si="6"/>
         <v>IMG22</v>
       </c>
-      <c r="B31" s="111" t="s">
+      <c r="B31" s="80" t="s">
         <v>235</v>
       </c>
       <c r="C31" s="20" t="str">
@@ -3965,7 +3965,7 @@
         <f ca="1">IF(OR($B31&lt;&gt;"",$J31&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E31,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E31,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J31" s="107" t="s">
+      <c r="J31" s="76" t="s">
         <v>236</v>
       </c>
       <c r="K31" s="64" t="s">
@@ -3977,7 +3977,7 @@
         <f t="shared" si="6"/>
         <v>IMG23</v>
       </c>
-      <c r="B32" s="107" t="s">
+      <c r="B32" s="76" t="s">
         <v>238</v>
       </c>
       <c r="C32" s="20" t="str">
@@ -4006,7 +4006,7 @@
         <f ca="1">IF(OR($B32&lt;&gt;"",$J32&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E32,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E32,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J32" s="107" t="s">
+      <c r="J32" s="76" t="s">
         <v>239</v>
       </c>
       <c r="K32" s="64"/>
@@ -4016,7 +4016,7 @@
         <f t="shared" si="6"/>
         <v>IMG24</v>
       </c>
-      <c r="B33" s="107" t="s">
+      <c r="B33" s="76" t="s">
         <v>240</v>
       </c>
       <c r="C33" s="20" t="str">
@@ -4045,7 +4045,7 @@
         <f ca="1">IF(OR($B33&lt;&gt;"",$J33&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E33,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E33,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J33" s="107" t="s">
+      <c r="J33" s="76" t="s">
         <v>241</v>
       </c>
       <c r="K33" s="64"/>
@@ -4055,7 +4055,7 @@
         <f t="shared" si="6"/>
         <v>IMG25</v>
       </c>
-      <c r="B34" s="107" t="s">
+      <c r="B34" s="76" t="s">
         <v>242</v>
       </c>
       <c r="C34" s="20" t="str">
@@ -4084,7 +4084,7 @@
         <f ca="1">IF(OR($B34&lt;&gt;"",$J34&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E34,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E34,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J34" s="107" t="s">
+      <c r="J34" s="76" t="s">
         <v>243</v>
       </c>
       <c r="K34" s="64"/>
@@ -4095,7 +4095,7 @@
         <f t="shared" si="6"/>
         <v>IMG26</v>
       </c>
-      <c r="B35" s="107" t="s">
+      <c r="B35" s="76" t="s">
         <v>244</v>
       </c>
       <c r="C35" s="20" t="str">
@@ -4124,7 +4124,7 @@
         <f ca="1">IF(OR($B35&lt;&gt;"",$J35&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E35,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E35,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J35" s="107" t="s">
+      <c r="J35" s="76" t="s">
         <v>245</v>
       </c>
       <c r="K35" s="65"/>
@@ -4135,7 +4135,7 @@
         <f t="shared" si="6"/>
         <v>IMG27</v>
       </c>
-      <c r="B36" s="107" t="s">
+      <c r="B36" s="76" t="s">
         <v>246</v>
       </c>
       <c r="C36" s="20" t="str">
@@ -4164,7 +4164,7 @@
         <f ca="1">IF(OR($B36&lt;&gt;"",$J36&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E36,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E36,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J36" s="107" t="s">
+      <c r="J36" s="76" t="s">
         <v>247</v>
       </c>
       <c r="K36" s="65"/>
@@ -4175,7 +4175,7 @@
         <f t="shared" si="6"/>
         <v>IMG28</v>
       </c>
-      <c r="B37" s="107" t="s">
+      <c r="B37" s="76" t="s">
         <v>248</v>
       </c>
       <c r="C37" s="20" t="str">
@@ -4204,7 +4204,7 @@
         <f ca="1">IF(OR($B37&lt;&gt;"",$J37&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E37,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E37,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J37" s="107" t="s">
+      <c r="J37" s="76" t="s">
         <v>249</v>
       </c>
       <c r="K37" s="65"/>
@@ -4214,7 +4214,7 @@
         <f t="shared" si="6"/>
         <v>IMG29</v>
       </c>
-      <c r="B38" s="107" t="s">
+      <c r="B38" s="76" t="s">
         <v>250</v>
       </c>
       <c r="C38" s="20" t="str">
@@ -4243,7 +4243,7 @@
         <f ca="1">IF(OR($B38&lt;&gt;"",$J38&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E38,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E38,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J38" s="107" t="s">
+      <c r="J38" s="76" t="s">
         <v>251</v>
       </c>
       <c r="K38" s="65"/>
@@ -4253,7 +4253,7 @@
         <f t="shared" si="6"/>
         <v>IMG30</v>
       </c>
-      <c r="B39" s="107" t="s">
+      <c r="B39" s="76" t="s">
         <v>252</v>
       </c>
       <c r="C39" s="20" t="str">
@@ -4282,7 +4282,7 @@
         <f ca="1">IF(OR($B39&lt;&gt;"",$J39&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E39,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E39,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J39" s="107" t="s">
+      <c r="J39" s="76" t="s">
         <v>253</v>
       </c>
       <c r="K39" s="65"/>
@@ -4292,7 +4292,7 @@
         <f t="shared" si="6"/>
         <v>IMG31</v>
       </c>
-      <c r="B40" s="107" t="s">
+      <c r="B40" s="76" t="s">
         <v>254</v>
       </c>
       <c r="C40" s="20" t="str">
@@ -4331,7 +4331,7 @@
         <f t="shared" si="6"/>
         <v>IMG32</v>
       </c>
-      <c r="B41" s="107" t="s">
+      <c r="B41" s="76" t="s">
         <v>256</v>
       </c>
       <c r="C41" s="20" t="str">
@@ -4360,7 +4360,7 @@
         <f ca="1">IF(OR($B41&lt;&gt;"",$J41&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E41,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E41,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J41" s="107" t="s">
+      <c r="J41" s="76" t="s">
         <v>257</v>
       </c>
       <c r="K41" s="65"/>
@@ -4370,7 +4370,7 @@
         <f t="shared" si="6"/>
         <v>IMG33</v>
       </c>
-      <c r="B42" s="108" t="s">
+      <c r="B42" s="77" t="s">
         <v>258</v>
       </c>
       <c r="C42" s="20" t="str">
@@ -4399,7 +4399,7 @@
         <f ca="1">IF(OR($B42&lt;&gt;"",$J42&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E42,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E42,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J42" s="107" t="s">
+      <c r="J42" s="76" t="s">
         <v>259</v>
       </c>
       <c r="K42" s="65" t="s">
@@ -4411,7 +4411,7 @@
         <f t="shared" si="6"/>
         <v>IMG34</v>
       </c>
-      <c r="B43" s="107" t="s">
+      <c r="B43" s="76" t="s">
         <v>261</v>
       </c>
       <c r="C43" s="20" t="str">
@@ -4450,7 +4450,7 @@
         <f t="shared" si="6"/>
         <v>IMG35</v>
       </c>
-      <c r="B44" s="107" t="s">
+      <c r="B44" s="76" t="s">
         <v>263</v>
       </c>
       <c r="C44" s="20" t="str">
@@ -4479,7 +4479,7 @@
         <f ca="1">IF(OR($B44&lt;&gt;"",$J44&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E44,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E44,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J44" s="107" t="s">
+      <c r="J44" s="76" t="s">
         <v>264</v>
       </c>
       <c r="K44" s="65"/>
@@ -4489,7 +4489,7 @@
         <f t="shared" si="6"/>
         <v>IMG36</v>
       </c>
-      <c r="B45" s="107" t="s">
+      <c r="B45" s="76" t="s">
         <v>265</v>
       </c>
       <c r="C45" s="20" t="str">
@@ -4518,7 +4518,7 @@
         <f ca="1">IF(OR($B45&lt;&gt;"",$J45&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E45,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E45,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J45" s="107" t="s">
+      <c r="J45" s="76" t="s">
         <v>266</v>
       </c>
       <c r="K45" s="65"/>
@@ -4528,7 +4528,7 @@
         <f t="shared" si="6"/>
         <v>IMG37</v>
       </c>
-      <c r="B46" s="107" t="s">
+      <c r="B46" s="76" t="s">
         <v>267</v>
       </c>
       <c r="C46" s="20" t="str">
@@ -4557,7 +4557,7 @@
         <f ca="1">IF(OR($B46&lt;&gt;"",$J46&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E46,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E46,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J46" s="107" t="s">
+      <c r="J46" s="76" t="s">
         <v>268</v>
       </c>
       <c r="K46" s="65"/>
@@ -4567,7 +4567,7 @@
         <f t="shared" si="6"/>
         <v>IMG38</v>
       </c>
-      <c r="B47" s="107" t="s">
+      <c r="B47" s="76" t="s">
         <v>269</v>
       </c>
       <c r="C47" s="20" t="str">
@@ -4596,7 +4596,7 @@
         <f ca="1">IF(OR($B47&lt;&gt;"",$J47&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E47,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E47,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J47" s="107" t="s">
+      <c r="J47" s="76" t="s">
         <v>270</v>
       </c>
       <c r="K47" s="65"/>
@@ -4606,7 +4606,7 @@
         <f t="shared" si="6"/>
         <v>IMG39</v>
       </c>
-      <c r="B48" s="107" t="s">
+      <c r="B48" s="76" t="s">
         <v>271</v>
       </c>
       <c r="C48" s="20" t="str">
@@ -4635,7 +4635,7 @@
         <f ca="1">IF(OR($B48&lt;&gt;"",$J48&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E48,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E48,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J48" s="107" t="s">
+      <c r="J48" s="76" t="s">
         <v>272</v>
       </c>
       <c r="K48" s="65"/>
@@ -4645,7 +4645,7 @@
         <f t="shared" si="6"/>
         <v>IMG40</v>
       </c>
-      <c r="B49" s="107" t="s">
+      <c r="B49" s="76" t="s">
         <v>273</v>
       </c>
       <c r="C49" s="20" t="str">
@@ -4674,7 +4674,7 @@
         <f ca="1">IF(OR($B49&lt;&gt;"",$J49&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E49,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E49,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J49" s="107" t="s">
+      <c r="J49" s="76" t="s">
         <v>274</v>
       </c>
       <c r="K49" s="65"/>
@@ -4684,7 +4684,7 @@
         <f t="shared" si="6"/>
         <v>IMG41</v>
       </c>
-      <c r="B50" s="107" t="s">
+      <c r="B50" s="76" t="s">
         <v>275</v>
       </c>
       <c r="C50" s="20" t="str">
@@ -4713,7 +4713,7 @@
         <f ca="1">IF(OR($B50&lt;&gt;"",$J50&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E50,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E50,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J50" s="107" t="s">
+      <c r="J50" s="76" t="s">
         <v>276</v>
       </c>
       <c r="K50" s="65"/>
@@ -6588,25 +6588,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.5" thickBot="1">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="96" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="93"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="98"/>
     </row>
     <row r="2" spans="1:11" ht="15.75">
       <c r="A2" s="30" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="31"/>
-      <c r="C2" s="94" t="s">
+      <c r="C2" s="99" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="95"/>
-      <c r="E2" s="96"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="101"/>
       <c r="F2" s="32"/>
     </row>
     <row r="3" spans="1:11" ht="60">
@@ -6614,11 +6614,11 @@
         <v>43</v>
       </c>
       <c r="B3" s="31"/>
-      <c r="C3" s="100" t="s">
+      <c r="C3" s="105" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="101"/>
-      <c r="E3" s="102"/>
+      <c r="D3" s="106"/>
+      <c r="E3" s="107"/>
       <c r="F3" s="32"/>
       <c r="H3" s="22" t="s">
         <v>18</v>
@@ -6669,11 +6669,11 @@
       <c r="C5" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="103" t="str">
+      <c r="D5" s="108" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_CO")</f>
         <v>LE_07_04_CO</v>
       </c>
-      <c r="E5" s="104"/>
+      <c r="E5" s="109"/>
       <c r="F5" s="32"/>
       <c r="H5" s="22" t="s">
         <v>22</v>
@@ -6718,12 +6718,12 @@
       <c r="C7" s="59" t="s">
         <v>119</v>
       </c>
-      <c r="D7" s="89" t="str">
+      <c r="D7" s="94" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D5,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_CO.xls</v>
       </c>
-      <c r="E7" s="89"/>
-      <c r="F7" s="90"/>
+      <c r="E7" s="94"/>
+      <c r="F7" s="95"/>
       <c r="H7" s="22" t="s">
         <v>24</v>
       </c>
@@ -6817,14 +6817,14 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.75">
-      <c r="A13" s="91" t="s">
+      <c r="A13" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="92"/>
-      <c r="C13" s="92"/>
-      <c r="D13" s="92"/>
-      <c r="E13" s="92"/>
-      <c r="F13" s="93"/>
+      <c r="B13" s="97"/>
+      <c r="C13" s="97"/>
+      <c r="D13" s="97"/>
+      <c r="E13" s="97"/>
+      <c r="F13" s="98"/>
       <c r="I13" s="22" t="s">
         <v>33</v>
       </c>
@@ -6857,12 +6857,12 @@
         <v>46</v>
       </c>
       <c r="B15" s="31"/>
-      <c r="C15" s="94" t="s">
+      <c r="C15" s="99" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="95"/>
-      <c r="E15" s="95"/>
-      <c r="F15" s="96"/>
+      <c r="D15" s="100"/>
+      <c r="E15" s="100"/>
+      <c r="F15" s="101"/>
       <c r="J15" s="22">
         <v>12</v>
       </c>
@@ -6902,12 +6902,12 @@
       <c r="C17" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="97" t="str">
+      <c r="D17" s="102" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_",K45)</f>
         <v>LE_07_04_REC10</v>
       </c>
-      <c r="E17" s="98"/>
-      <c r="F17" s="99"/>
+      <c r="E17" s="103"/>
+      <c r="F17" s="104"/>
       <c r="J17" s="22">
         <v>14</v>
       </c>
@@ -6923,12 +6923,12 @@
       <c r="C18" s="59" t="s">
         <v>120</v>
       </c>
-      <c r="D18" s="89" t="str">
+      <c r="D18" s="94" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D17,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_REC10.xls</v>
       </c>
-      <c r="E18" s="89"/>
-      <c r="F18" s="90"/>
+      <c r="E18" s="94"/>
+      <c r="F18" s="95"/>
       <c r="J18" s="22">
         <v>15</v>
       </c>
@@ -7319,40 +7319,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="111" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="106" t="s">
+      <c r="B1" s="111" t="s">
         <v>149</v>
       </c>
-      <c r="C1" s="106" t="s">
+      <c r="C1" s="111" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="106" t="s">
+      <c r="D1" s="111" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="106" t="s">
+      <c r="E1" s="111" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="106" t="s">
+      <c r="F1" s="111" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="106" t="s">
+      <c r="G1" s="111" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="105" t="s">
+      <c r="H1" s="110" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="105"/>
+      <c r="I1" s="110"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="106"/>
-      <c r="B2" s="106"/>
-      <c r="C2" s="106"/>
-      <c r="D2" s="106"/>
-      <c r="E2" s="106"/>
-      <c r="F2" s="106"/>
-      <c r="G2" s="106"/>
+      <c r="A2" s="111"/>
+      <c r="B2" s="111"/>
+      <c r="C2" s="111"/>
+      <c r="D2" s="111"/>
+      <c r="E2" s="111"/>
+      <c r="F2" s="111"/>
+      <c r="G2" s="111"/>
       <c r="H2" s="39" t="s">
         <v>65</v>
       </c>

</xml_diff>